<commit_message>
added netinc, hispanic  fixed (life is sad)
</commit_message>
<xml_diff>
--- a/data-raw/it_us/us/american_comunity_survey_2018/age_sex/to_select_age_sex.xlsx
+++ b/data-raw/it_us/us/american_comunity_survey_2018/age_sex/to_select_age_sex.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heverz/Documents/R_projects/extractus/data-raw/american_comunity_survey_2018/age_sex/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heverz/Documents/R_projects/covid19census/data-raw/it_us/us/american_comunity_survey_2018/age_sex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290726ED-0498-FF46-92C3-C1C22050FACD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9B6D44-247C-6B44-872C-6D5E1948D3DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1544,12 +1544,12 @@
   <dimension ref="A1:B114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
added age summary indicators
</commit_message>
<xml_diff>
--- a/data-raw/it_us/us/american_comunity_survey_2018/age_sex/to_select_age_sex.xlsx
+++ b/data-raw/it_us/us/american_comunity_survey_2018/age_sex/to_select_age_sex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heverz/Documents/R_projects/covid19census/data-raw/it_us/us/american_comunity_survey_2018/age_sex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9B6D44-247C-6B44-872C-6D5E1948D3DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E559EB-0C38-F448-ACED-950351446422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="241">
   <si>
     <t>new_names</t>
   </si>
@@ -701,6 +701,48 @@
   </si>
   <si>
     <t>geographic_area_name</t>
+  </si>
+  <si>
+    <t>estimate_total_total_population_summary_indicators_median_age_years</t>
+  </si>
+  <si>
+    <t>estimate_male_total_population_summary_indicators_median_age_years</t>
+  </si>
+  <si>
+    <t>estimate_female_total_population_summary_indicators_median_age_years</t>
+  </si>
+  <si>
+    <t>estimate_total_total_population_summary_indicators_sex_ratio_males_per_100_females</t>
+  </si>
+  <si>
+    <t>estimate_total_total_population_summary_indicators_age_dependency_ratio</t>
+  </si>
+  <si>
+    <t>estimate_total_total_population_summary_indicators_old_age_dependency_ratio</t>
+  </si>
+  <si>
+    <t>estimate_total_total_population_summary_indicators_child_dependency_ratio</t>
+  </si>
+  <si>
+    <t>median_age</t>
+  </si>
+  <si>
+    <t>median_age_male</t>
+  </si>
+  <si>
+    <t>median_age_female</t>
+  </si>
+  <si>
+    <t>sex_ratio</t>
+  </si>
+  <si>
+    <t>age_dependency</t>
+  </si>
+  <si>
+    <t>old_age_dependency</t>
+  </si>
+  <si>
+    <t>child_dependency</t>
   </si>
 </sst>
 </file>
@@ -1541,13 +1583,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B114"/>
+  <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q42" sqref="Q42"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="194" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2461,6 +2506,62 @@
         <v>223</v>
       </c>
     </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>234</v>
+      </c>
+      <c r="B115" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>235</v>
+      </c>
+      <c r="B116" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>236</v>
+      </c>
+      <c r="B117" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>237</v>
+      </c>
+      <c r="B118" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>238</v>
+      </c>
+      <c r="B119" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>239</v>
+      </c>
+      <c r="B120" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>240</v>
+      </c>
+      <c r="B121" t="s">
+        <v>233</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>